<commit_message>
Atualização dos dados extraídos e scripts de extração/ex consolidador
</commit_message>
<xml_diff>
--- a/scraper-completo/DADOS EXTRAIDOS/consorcio_contemplado_base.xlsx
+++ b/scraper-completo/DADOS EXTRAIDOS/consorcio_contemplado_base.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CS036</t>
+          <t>CS119</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -510,22 +510,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 70.000,00</t>
+          <t>R$ 69.600,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 42.500,00</t>
+          <t>R$ 22.480,00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>193</t>
+          <t>138</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>193x R$ 472,00</t>
+          <t>138x R$ 479,00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -544,7 +544,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CS037</t>
+          <t>CS120</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -554,22 +554,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 111.000,00</t>
+          <t>R$ 70.200,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 67.550,00</t>
+          <t>R$ 44.510,00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>192</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>74x R$ 1.387,00</t>
+          <t>192x R$ 399,00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -588,7 +588,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CS038</t>
+          <t>CS121</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -598,22 +598,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$ 120.000,00</t>
+          <t>R$ 110.000,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 75.000,00</t>
+          <t>R$ 70.500,00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>177</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>57x R$ 1.608,00</t>
+          <t>177x R$ 469,00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -632,7 +632,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CS039</t>
+          <t>CS122</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -642,17 +642,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 128.000,00</t>
+          <t>R$ 111.000,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 64.400,00</t>
+          <t>R$ 67.550,00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>53x R$ 2.333,00</t>
+          <t>73x R$ 1.387,00</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS040</t>
+          <t>CS123</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -686,17 +686,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 128.000,00</t>
+          <t>R$ 120.000,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 64.400,00</t>
+          <t>R$ 75.000,00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>56</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>53x R$ 2.342,00</t>
+          <t>56x R$ 1.608,00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -720,7 +720,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CS041</t>
+          <t>CS124</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -730,17 +730,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 137.000,00</t>
+          <t>R$ 128.000,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 73.850,00</t>
+          <t>R$ 64.400,00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>53x R$ 2.339,00</t>
+          <t>52x R$ 2.333,00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -764,7 +764,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CS042</t>
+          <t>CS125</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -774,22 +774,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 140.000,00</t>
+          <t>R$ 128.000,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 85.000,00</t>
+          <t>R$ 64.400,00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>193</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>193x R$ 944,00</t>
+          <t>52x R$ 2.342,00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -808,7 +808,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CS043</t>
+          <t>CS126</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -818,22 +818,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 150.000,00</t>
+          <t>R$ 132.000,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 75.500,00</t>
+          <t>R$ 31.600,00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>169</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>BP Consórcio</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>53x R$ 2.951,00</t>
+          <t>169x R$ 1.027,00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -852,7 +852,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CS044</t>
+          <t>CS127</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -862,22 +862,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 158.000,00</t>
+          <t>R$ 135.000,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 82.900,00</t>
+          <t>R$ 72.750,00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>92</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>53x R$ 2.894,00</t>
+          <t>92x R$ 1.395,00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -896,7 +896,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CS045</t>
+          <t>CS128</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -906,22 +906,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 187.200,00</t>
+          <t>R$ 137.000,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 104.360,00</t>
+          <t>R$ 73.850,00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>125x R$ 1.064,00</t>
+          <t>52x R$ 2.339,00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -940,7 +940,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CS046</t>
+          <t>CS129</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -950,22 +950,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 458.000,00</t>
+          <t>R$ 149.300,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 247.900,00</t>
+          <t>R$ 69.465,00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>136</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>118x R$ 3.222,00</t>
+          <t>136x R$ 854,00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -984,7 +984,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CS047</t>
+          <t>CS130</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -994,22 +994,22 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 525.000,00</t>
+          <t>R$ 150.000,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 246.250,00</t>
+          <t>R$ 75.500,00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>181x R$ 3.430,00</t>
+          <t>52x R$ 2.951,00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CS048</t>
+          <t>CS131</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1038,17 +1038,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>R$ 543.000,00</t>
+          <t>R$ 153.000,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 272.150,00</t>
+          <t>R$ 83.650,00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>83</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>145x R$ 4.370,00</t>
+          <t>83x R$ 1.845,00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1072,7 +1072,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CS049</t>
+          <t>CS132</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>R$ 1.334.000,00</t>
+          <t>R$ 158.000,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 665.700,00</t>
+          <t>R$ 82.900,00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>52</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>145x R$ 10.952,00</t>
+          <t>52x R$ 2.894,00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1116,32 +1116,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CS050</t>
+          <t>CS133</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 6.800,00</t>
+          <t>R$ 187.200,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R$ 2.840,00</t>
+          <t>R$ 104.360,00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>124</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>59x R$ 90,00</t>
+          <t>124x R$ 1.064,00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -1160,32 +1160,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CS051</t>
+          <t>CS134</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 9.900,00</t>
+          <t>R$ 212.000,00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R$ 5.995,00</t>
+          <t>R$ 131.600,00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>192</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>34x R$ 134,00</t>
+          <t>192x R$ 1.342,00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1204,32 +1204,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CS052</t>
+          <t>CS135</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 18.700,00</t>
+          <t>R$ 219.000,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 8.935,00</t>
+          <t>R$ 140.950,00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>177</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>63x R$ 310,00</t>
+          <t>177x R$ 938,00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1248,32 +1248,32 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CS053</t>
+          <t>CS136</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>R$ 31.250,00</t>
+          <t>R$ 474.300,00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R$ 13.562,50</t>
+          <t>R$ 258.715,00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>105</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>44x R$ 634,00</t>
+          <t>105x R$ 3.603,00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1292,32 +1292,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CS054</t>
+          <t>CS137</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>R$ 35.000,00</t>
+          <t>R$ 527.000,00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R$ 13.750,00</t>
+          <t>R$ 255.350,00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>180</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>37x R$ 1.267,00</t>
+          <t>180x R$ 3.430,00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1336,32 +1336,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CS055</t>
+          <t>CS138</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>R$ 40.100,00</t>
+          <t>R$ 546.000,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>R$ 14.005,00</t>
+          <t>R$ 286.300,00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>144</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>30x R$ 1.645,00</t>
+          <t>144x R$ 4.370,00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1380,32 +1380,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CS056</t>
+          <t>CS139</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Veículos</t>
+          <t>Imóveis</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>R$ 58.000,00</t>
+          <t>R$ 1.334.000,00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R$ 21.900,00</t>
+          <t>R$ 665.700,00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>144</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>33x R$ 2.045,00</t>
+          <t>144x R$ 10.952,00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CS057</t>
+          <t>CS140</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1434,22 +1434,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>R$ 109.000,00</t>
+          <t>R$ 6.800,00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R$ 64.450,00</t>
+          <t>R$ 2.840,00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>58</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>50x R$ 1.657,00</t>
+          <t>58x R$ 90,00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1468,7 +1468,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CS058</t>
+          <t>CS141</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1478,22 +1478,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>R$ 124.300,00</t>
+          <t>R$ 10.000,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>R$ 68.215,00</t>
+          <t>R$ 6.000,00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>65x R$ 1.877,00</t>
+          <t>33x R$ 135,00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1512,7 +1512,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CS059</t>
+          <t>CS142</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1522,12 +1522,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>R$ 126.000,00</t>
+          <t>R$ 18.600,00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>R$ 61.300,00</t>
+          <t>R$ 11.930,00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>53x R$ 2.380,00</t>
+          <t>53x R$ 365,00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1556,7 +1556,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CS060</t>
+          <t>CS143</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1566,22 +1566,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>R$ 126.000,00</t>
+          <t>R$ 31.250,00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>R$ 82.300,00</t>
+          <t>R$ 13.562,50</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>43</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>65x R$ 1.665,00</t>
+          <t>43x R$ 634,00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1600,7 +1600,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CS061</t>
+          <t>CS144</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1610,22 +1610,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>R$ 128.600,00</t>
+          <t>R$ 35.600,00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R$ 75.430,00</t>
+          <t>R$ 19.780,00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>44</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>64x R$ 1.645,00</t>
+          <t>44x R$ 709,00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1644,7 +1644,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CS062</t>
+          <t>CS145</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1654,17 +1654,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>R$ 132.000,00</t>
+          <t>R$ 40.700,00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R$ 64.600,00</t>
+          <t>R$ 23.035,00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>54x R$ 2.455,00</t>
+          <t>49x R$ 847,00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1688,7 +1688,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CS063</t>
+          <t>CS146</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1698,17 +1698,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>R$ 140.000,00</t>
+          <t>R$ 41.000,00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>R$ 65.000,00</t>
+          <t>R$ 24.050,00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>42x R$ 3.678,00</t>
+          <t>49x R$ 825,00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CS064</t>
+          <t>CS147</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1742,22 +1742,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>R$ 199.600,00</t>
+          <t>R$ 67.700,00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>R$ 108.980,00</t>
+          <t>R$ 35.385,00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>54</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>67x R$ 2.904,00</t>
+          <t>54x R$ 1.250,00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1776,7 +1776,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CS065</t>
+          <t>CS148</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1786,22 +1786,22 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>R$ 206.100,00</t>
+          <t>R$ 70.900,00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>R$ 109.305,00</t>
+          <t>R$ 26.545,00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>65x R$ 2.966,00</t>
+          <t>37x R$ 2.424,00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CS066</t>
+          <t>CS149</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1830,17 +1830,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>R$ 209.000,00</t>
+          <t>R$ 106.300,00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>R$ 88.450,00</t>
+          <t>R$ 38.315,00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>58x R$ 3.630,00</t>
+          <t>37x R$ 3.636,00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1864,7 +1864,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CS067</t>
+          <t>CS150</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1874,22 +1874,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>R$ 309.000,00</t>
+          <t>R$ 109.000,00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>R$ 125.450,00</t>
+          <t>R$ 67.450,00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>48x R$ 6.190,00</t>
+          <t>49x R$ 1.657,00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1908,7 +1908,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CS068</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1918,22 +1918,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>R$ 310.000,00</t>
+          <t>R$ 118.600,00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>R$ 125.500,00</t>
+          <t>R$ 69.930,00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Unicoob (Sicoob)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>48x R$ 6.079,00</t>
+          <t>34x R$ 2.018,00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1952,7 +1952,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CS069</t>
+          <t>CS152</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1962,22 +1962,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>R$ 470.000,00</t>
+          <t>R$ 119.000,00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>R$ 263.500,00</t>
+          <t>R$ 67.950,00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>49x R$ 6.820,00</t>
+          <t>48x R$ 2.250,00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1996,7 +1996,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CS070</t>
+          <t>CS153</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2006,17 +2006,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>R$ 619.000,00</t>
+          <t>R$ 121.300,00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>R$ 250.950,00</t>
+          <t>R$ 41.065,00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>29</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2031,11 +2031,583 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>48x R$ 12.269,00</t>
+          <t>29x R$ 4.932,00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CS154</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>R$ 125.000,00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>R$ 68.250,00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>64x R$ 1.877,00</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CS155</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>R$ 129.000,00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>R$ 78.450,00</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>64x R$ 1.665,00</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CS156</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>R$ 140.000,00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>R$ 65.000,00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>41x R$ 3.678,00</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CS157</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>R$ 201.000,00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>R$ 105.050,00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>66x R$ 2.902,00</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CS158</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>R$ 207.000,00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>R$ 105.350,00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>64x R$ 2.966,00</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CS159</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>R$ 209.000,00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>R$ 99.450,00</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>57x R$ 3.590,00</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CS160</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>R$ 210.000,00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>R$ 99.500,00</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>57x R$ 3.630,00</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>R$ 254.000,00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>R$ 144.700,00</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>64x R$ 3.520,00</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CS162</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>R$ 310.000,00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>R$ 130.500,00</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>47x R$ 6.190,00</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CS163</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>R$ 312.000,00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>R$ 132.600,00</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>47x R$ 6.079,00</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CS164</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>R$ 332.200,00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>R$ 171.610,00</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Porto Seguro</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>64x R$ 4.841,00</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CS165</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>R$ 471.000,00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>R$ 263.550,00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>48x R$ 6.820,00</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CS166</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Veículos</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>R$ 620.000,00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>R$ 261.000,00</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Itaú</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Disponível</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>47x R$ 12.269,00</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Atualiza arquivos de dados extraídos
</commit_message>
<xml_diff>
--- a/scraper-completo/DADOS EXTRAIDOS/consorcio_contemplado_base.xlsx
+++ b/scraper-completo/DADOS EXTRAIDOS/consorcio_contemplado_base.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="15" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
@@ -500,7 +500,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CS167</t>
+          <t>CS210</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -510,22 +510,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 69.600,00</t>
+          <t>R$ 101.300,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 22.480,00</t>
+          <t>R$ 56.065,00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>154</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>138x R$ 479,00</t>
+          <t>154x R$ 651,00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -544,7 +544,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CS168</t>
+          <t>CS211</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -554,17 +554,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 70.200,00</t>
+          <t>R$ 126.900,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 44.510,00</t>
+          <t>R$ 68.345,00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>93</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>192x R$ 399,00</t>
+          <t>93x R$ 1.460,00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -588,7 +588,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CS169</t>
+          <t>CS212</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -598,17 +598,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$ 110.000,00</t>
+          <t>R$ 135.000,00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 70.500,00</t>
+          <t>R$ 72.750,00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>177</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>177x R$ 469,00</t>
+          <t>91x R$ 1.395,00</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -632,7 +632,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CS170</t>
+          <t>CS213</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -642,22 +642,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 111.000,00</t>
+          <t>R$ 135.300,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 67.550,00</t>
+          <t>R$ 72.765,00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>73x R$ 1.387,00</t>
+          <t>91x R$ 1.395,00</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -676,7 +676,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS171</t>
+          <t>CS214</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -686,22 +686,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 120.000,00</t>
+          <t>R$ 153.000,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 75.000,00</t>
+          <t>R$ 83.650,00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>82</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>56x R$ 1.608,00</t>
+          <t>82x R$ 1.845,00</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -720,7 +720,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CS172</t>
+          <t>CS215</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -730,22 +730,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 128.000,00</t>
+          <t>R$ 154.000,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 64.400,00</t>
+          <t>R$ 66.700,00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>145</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>52x R$ 2.333,00</t>
+          <t>145x R$ 1.303,00</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -764,7 +764,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CS173</t>
+          <t>CS216</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -774,17 +774,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 128.000,00</t>
+          <t>R$ 164.100,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 64.400,00</t>
+          <t>R$ 97.205,00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>162</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>52x R$ 2.342,00</t>
+          <t>162x R$ 1.203,00</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -808,7 +808,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CS174</t>
+          <t>CS217</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -818,22 +818,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 132.000,00</t>
+          <t>R$ 168.500,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 31.600,00</t>
+          <t>R$ 93.425,00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>139</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BP Consórcio</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>169x R$ 1.027,00</t>
+          <t>139x R$ 1.187,00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -852,7 +852,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CS175</t>
+          <t>CS218</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -862,22 +862,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 135.000,00</t>
+          <t>R$ 218.800,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 72.750,00</t>
+          <t>R$ 125.940,00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>128</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>92x R$ 1.395,00</t>
+          <t>128x R$ 2.157,00</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -896,7 +896,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CS176</t>
+          <t>CS219</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -906,17 +906,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 137.000,00</t>
+          <t>R$ 218.800,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 73.850,00</t>
+          <t>R$ 125.940,00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>128</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>52x R$ 2.339,00</t>
+          <t>128x R$ 2.157,00</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -940,7 +940,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CS177</t>
+          <t>CS220</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -950,17 +950,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 150.000,00</t>
+          <t>R$ 257.200,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 75.500,00</t>
+          <t>R$ 157.860,00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>52x R$ 2.951,00</t>
+          <t>99x R$ 2.459,00</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -984,7 +984,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CS178</t>
+          <t>CS221</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -994,17 +994,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 153.000,00</t>
+          <t>R$ 433.400,00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 83.650,00</t>
+          <t>R$ 280.670,00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>144</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>83x R$ 1.845,00</t>
+          <t>144x R$ 2.632,00</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CS179</t>
+          <t>CS222</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1038,17 +1038,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>R$ 158.000,00</t>
+          <t>R$ 602.000,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 82.900,00</t>
+          <t>R$ 179.100,00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>52x R$ 2.894,00</t>
+          <t>39x R$ 19.774,00</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1072,7 +1072,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CS180</t>
+          <t>CS223</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1082,22 +1082,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>R$ 187.200,00</t>
+          <t>R$ 655.000,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 104.360,00</t>
+          <t>R$ 411.750,00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>124x R$ 1.064,00</t>
+          <t>91x R$ 4.162,00</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
@@ -1116,7 +1116,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CS181</t>
+          <t>CS224</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1126,22 +1126,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 212.000,00</t>
+          <t>R$ 676.000,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R$ 131.600,00</t>
+          <t>R$ 402.800,00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>192x R$ 1.342,00</t>
+          <t>73x R$ 5.557,00</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -1160,7 +1160,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CS182</t>
+          <t>CS225</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1170,22 +1170,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 219.000,00</t>
+          <t>R$ 881.200,00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R$ 140.950,00</t>
+          <t>R$ 403.060,00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>177</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>177x R$ 938,00</t>
+          <t>73x R$ 15.493,00</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1204,7 +1204,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CS183</t>
+          <t>CS226</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1214,22 +1214,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 474.300,00</t>
+          <t>R$ 1.557.100,00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 258.715,00</t>
+          <t>R$ 776.855,00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>105x R$ 3.603,00</t>
+          <t>73x R$ 21.050,00</t>
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
@@ -1248,27 +1248,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CS184</t>
+          <t>CS227</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>R$ 1.334.000,00</t>
+          <t>R$ 6.800,00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R$ 665.700,00</t>
+          <t>R$ 2.840,00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>57</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>144x R$ 10.952,00</t>
+          <t>57x R$ 90,00</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1292,7 +1292,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CS185</t>
+          <t>CS228</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1302,22 +1302,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>R$ 6.800,00</t>
+          <t>R$ 10.000,00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R$ 2.840,00</t>
+          <t>R$ 6.000,00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>32</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>57x R$ 90,00</t>
+          <t>32x R$ 135,00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr"/>
@@ -1336,7 +1336,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CS186</t>
+          <t>CS229</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1346,22 +1346,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>R$ 10.000,00</t>
+          <t>R$ 38.000,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>R$ 6.000,00</t>
+          <t>R$ 8.900,00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>32x R$ 135,00</t>
+          <t>33x R$ 1.292,00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr"/>
@@ -1380,7 +1380,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CS187</t>
+          <t>CS230</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1390,22 +1390,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>R$ 31.250,00</t>
+          <t>R$ 110.300,00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R$ 13.562,50</t>
+          <t>R$ 66.515,00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>49</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>43x R$ 634,00</t>
+          <t>49x R$ 1.636,00</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CS188</t>
+          <t>CS231</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1434,22 +1434,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>R$ 70.900,00</t>
+          <t>R$ 110.300,00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R$ 26.545,00</t>
+          <t>R$ 68.515,00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>37x R$ 2.424,00</t>
+          <t>48x R$ 1.636,00</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
@@ -1468,7 +1468,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CS189</t>
+          <t>CS232</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1478,17 +1478,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>R$ 106.300,00</t>
+          <t>R$ 112.000,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>R$ 38.315,00</t>
+          <t>R$ 54.600,00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>37x R$ 3.636,00</t>
+          <t>51x R$ 2.240,00</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1512,7 +1512,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CS190</t>
+          <t>CS233</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1522,17 +1522,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>R$ 109.000,00</t>
+          <t>R$ 125.200,00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>R$ 67.450,00</t>
+          <t>R$ 64.260,00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>64</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>49x R$ 1.657,00</t>
+          <t>64x R$ 1.875,00</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1556,7 +1556,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CS191</t>
+          <t>CS234</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1566,22 +1566,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>R$ 118.600,00</t>
+          <t>R$ 126.100,00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>R$ 69.930,00</t>
+          <t>R$ 64.305,00</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>63</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Unicoob (Sicoob)</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>34x R$ 2.018,00</t>
+          <t>63x R$ 1.874,00</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1600,7 +1600,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CS192</t>
+          <t>CS235</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1610,17 +1610,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>R$ 119.000,00</t>
+          <t>R$ 127.500,00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R$ 67.950,00</t>
+          <t>R$ 68.375,00</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>48x R$ 2.250,00</t>
+          <t>62x R$ 2.030,00</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1644,7 +1644,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CS193</t>
+          <t>CS236</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1654,17 +1654,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>R$ 121.300,00</t>
+          <t>R$ 128.000,00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R$ 41.065,00</t>
+          <t>R$ 55.400,00</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>29x R$ 4.932,00</t>
+          <t>39x R$ 3.590,00</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1688,7 +1688,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CS194</t>
+          <t>CS237</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1698,22 +1698,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>R$ 125.000,00</t>
+          <t>R$ 128.000,00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>R$ 68.250,00</t>
+          <t>R$ 55.400,00</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>64x R$ 1.877,00</t>
+          <t>39x R$ 3.590,00</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CS195</t>
+          <t>CS238</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1742,22 +1742,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>R$ 126.000,00</t>
+          <t>R$ 135.400,00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>R$ 60.300,00</t>
+          <t>R$ 65.770,00</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>66</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>54x R$ 2.650,00</t>
+          <t>66x R$ 2.125,00</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1776,7 +1776,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CS196</t>
+          <t>CS239</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1786,17 +1786,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>R$ 129.000,00</t>
+          <t>R$ 137.000,00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>R$ 78.450,00</t>
+          <t>R$ 78.850,00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>65</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>64x R$ 1.665,00</t>
+          <t>65x R$ 1.937,00</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CS197</t>
+          <t>CS240</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1830,22 +1830,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>R$ 131.000,00</t>
+          <t>R$ 161.000,00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>R$ 61.550,00</t>
+          <t>R$ 87.050,00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>66</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>53x R$ 2.670,00</t>
+          <t>66x R$ 1.856,00</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1864,7 +1864,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CS198</t>
+          <t>CS241</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1874,22 +1874,22 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>R$ 141.000,00</t>
+          <t>R$ 181.000,00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>R$ 62.050,00</t>
+          <t>R$ 93.050,00</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>62</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>40x R$ 3.543,00</t>
+          <t>62x R$ 2.678,00</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1908,7 +1908,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CS199</t>
+          <t>CS242</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1918,22 +1918,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>R$ 190.000,00</t>
+          <t>R$ 202.500,00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>R$ 93.500,00</t>
+          <t>R$ 103.125,00</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>65</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>56x R$ 3.300,00</t>
+          <t>65x R$ 2.902,00</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1952,7 +1952,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CS200</t>
+          <t>CS243</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1962,22 +1962,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>R$ 201.000,00</t>
+          <t>R$ 209.000,00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>R$ 105.050,00</t>
+          <t>R$ 99.450,00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>56</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>66x R$ 2.902,00</t>
+          <t>56x R$ 3.640,00</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1996,7 +1996,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CS201</t>
+          <t>CS244</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2006,22 +2006,22 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>R$ 207.000,00</t>
+          <t>R$ 210.000,00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>R$ 105.350,00</t>
+          <t>R$ 102.500,00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>56</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>64x R$ 2.966,00</t>
+          <t>56x R$ 3.637,00</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -2040,7 +2040,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CS202</t>
+          <t>CS245</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2050,17 +2050,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>R$ 254.000,00</t>
+          <t>R$ 216.300,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>R$ 144.700,00</t>
+          <t>R$ 83.815,00</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>64x R$ 3.520,00</t>
+          <t>48x R$ 4.835,00</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -2084,7 +2084,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CS203</t>
+          <t>CS246</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2094,22 +2094,22 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>R$ 257.000,00</t>
+          <t>R$ 221.400,00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>R$ 119.850,00</t>
+          <t>R$ 126.070,00</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>64</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>54x R$ 5.320,00</t>
+          <t>64x R$ 2.632,00</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -2128,7 +2128,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CS204</t>
+          <t>CS247</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2138,17 +2138,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>R$ 267.000,00</t>
+          <t>R$ 256.000,00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>R$ 118.350,00</t>
+          <t>R$ 110.800,00</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>39</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>54x R$ 5.320,00</t>
+          <t>39x R$ 7.180,00</t>
         </is>
       </c>
       <c r="I39" t="inlineStr"/>
@@ -2172,7 +2172,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CS205</t>
+          <t>CS248</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2182,17 +2182,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>R$ 267.000,00</t>
+          <t>R$ 471.000,00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>R$ 120.350,00</t>
+          <t>R$ 268.550,00</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>48</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2207,187 +2207,11 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>54x R$ 6.193,00</t>
+          <t>48x R$ 6.820,00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CS206</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Veículos</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>R$ 272.000,00</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>R$ 122.600,00</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Itaú</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Disponível</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>53x R$ 6.213,00</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CS207</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Veículos</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>R$ 332.200,00</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>R$ 171.610,00</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Porto Seguro</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Disponível</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>64x R$ 4.841,00</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CS208</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Veículos</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>R$ 398.000,00</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>R$ 174.900,00</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Itaú</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Disponível</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>53x R$ 8.863,00</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CS209</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Veículos</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>R$ 471.000,00</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>R$ 268.550,00</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Itaú</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Disponível</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>48x R$ 6.820,00</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>